<commit_message>
changes in many jsons
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/005.xlsx
+++ b/docs/STAFF-DATA/005.xlsx
@@ -704,7 +704,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -716,7 +716,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -783,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -796,6 +796,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -818,29 +821,29 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1150,24 +1153,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="29.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="19" width="53.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="17" width="29.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="18" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="18" width="53.14785714285715" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="19" width="36.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="18" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="20" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="48">
@@ -1202,71 +1205,71 @@
         <v>9</v>
       </c>
       <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
       <c r="R1" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
       <c r="R2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="88.5" customFormat="1" s="10">
-      <c r="A3" s="11" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="88.5" customFormat="1" s="11">
+      <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="12"/>
@@ -1276,19 +1279,19 @@
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
-      <c r="R3" s="6"/>
+      <c r="R3" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="88.5">
       <c r="A4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1300,7 +1303,7 @@
       <c r="G4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -1310,25 +1313,25 @@
         <v>33</v>
       </c>
       <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
       <c r="R4" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33.75">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="4"/>
@@ -1344,25 +1347,25 @@
         <v>40</v>
       </c>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
       <c r="R5" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33.75">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="4"/>
@@ -1378,25 +1381,25 @@
         <v>46</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
       <c r="R6" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="4"/>
@@ -1410,25 +1413,25 @@
         <v>51</v>
       </c>
       <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
       <c r="R7" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33.75">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="7" t="s">
         <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1438,7 +1441,7 @@
         <v>56</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="7" t="s">
         <v>57</v>
       </c>
       <c r="I8" s="4" t="s">
@@ -1448,25 +1451,25 @@
         <v>59</v>
       </c>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
       <c r="R8" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="47.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="7" t="s">
         <v>63</v>
       </c>
       <c r="E9" s="4"/>
@@ -1482,25 +1485,25 @@
         <v>66</v>
       </c>
       <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
       <c r="R9" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33.75">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E10" s="4"/>
@@ -1516,25 +1519,25 @@
         <v>72</v>
       </c>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
       <c r="R10" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="47.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E11" s="4"/>
@@ -1548,25 +1551,25 @@
         <v>77</v>
       </c>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
       <c r="R11" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33.75">
       <c r="A12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="7" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1586,25 +1589,25 @@
         <v>85</v>
       </c>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
       <c r="R12" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33.75">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="7" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1616,7 +1619,7 @@
       <c r="G13" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="7" t="s">
         <v>84</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -1626,25 +1629,25 @@
         <v>91</v>
       </c>
       <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
       <c r="R13" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="116.25">
       <c r="A14" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="7" t="s">
         <v>94</v>
       </c>
       <c r="E14" s="4"/>
@@ -1658,25 +1661,25 @@
         <v>96</v>
       </c>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
       <c r="R14" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="88.5">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E15" s="4"/>
@@ -1686,7 +1689,7 @@
       <c r="G15" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="7" t="s">
         <v>102</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -1696,25 +1699,25 @@
         <v>104</v>
       </c>
       <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
       <c r="R15" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="7" t="s">
         <v>107</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -1726,7 +1729,7 @@
       <c r="G16" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="7" t="s">
         <v>107</v>
       </c>
       <c r="I16" s="4" t="s">
@@ -1736,25 +1739,25 @@
         <v>110</v>
       </c>
       <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
       <c r="R16" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="7" t="s">
         <v>113</v>
       </c>
       <c r="E17" s="4"/>
@@ -1764,7 +1767,7 @@
       <c r="G17" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="7" t="s">
         <v>116</v>
       </c>
       <c r="I17" s="4" t="s">
@@ -1774,25 +1777,25 @@
         <v>117</v>
       </c>
       <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
       <c r="R17" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="7" t="s">
         <v>120</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -1810,25 +1813,25 @@
         <v>124</v>
       </c>
       <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
       <c r="R18" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="7" t="s">
         <v>127</v>
       </c>
       <c r="E19" s="4"/>
@@ -1842,25 +1845,25 @@
         <v>129</v>
       </c>
       <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
       <c r="R19" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="7" t="s">
         <v>132</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -1878,25 +1881,25 @@
         <v>136</v>
       </c>
       <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
       <c r="R20" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="7" t="s">
         <v>139</v>
       </c>
       <c r="E21" s="4"/>
@@ -1910,25 +1913,25 @@
         <v>141</v>
       </c>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
       <c r="R21" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="7" t="s">
         <v>144</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -1946,25 +1949,25 @@
         <v>148</v>
       </c>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
       <c r="R22" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="7" t="s">
         <v>151</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1974,7 +1977,7 @@
         <v>153</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="7" t="s">
         <v>154</v>
       </c>
       <c r="I23" s="4" t="s">
@@ -1984,25 +1987,25 @@
         <v>156</v>
       </c>
       <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
       <c r="R23" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="7" t="s">
         <v>159</v>
       </c>
       <c r="E24" s="4"/>
@@ -2016,25 +2019,25 @@
         <v>161</v>
       </c>
       <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
       <c r="R24" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -2052,25 +2055,25 @@
         <v>168</v>
       </c>
       <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
       <c r="R25" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="7" t="s">
         <v>84</v>
       </c>
       <c r="E26" s="4"/>
@@ -2084,25 +2087,25 @@
         <v>172</v>
       </c>
       <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
       <c r="R26" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="7" t="s">
         <v>84</v>
       </c>
       <c r="E27" s="4"/>
@@ -2116,25 +2119,25 @@
         <v>176</v>
       </c>
       <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
       <c r="R27" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="7" t="s">
         <v>179</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -2146,7 +2149,7 @@
       <c r="G28" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="7" t="s">
         <v>179</v>
       </c>
       <c r="I28" s="4" t="s">
@@ -2155,26 +2158,26 @@
       <c r="J28" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="K28" s="9"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
       <c r="R28" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="7" t="s">
         <v>184</v>
       </c>
       <c r="E29" s="4"/>
@@ -2188,22 +2191,22 @@
         <v>186</v>
       </c>
       <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
       <c r="R29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D30" s="12"/>
@@ -2216,22 +2219,22 @@
         <v>189</v>
       </c>
       <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
       <c r="R30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>191</v>
       </c>
       <c r="D31" s="12"/>
@@ -2244,22 +2247,22 @@
         <v>192</v>
       </c>
       <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
       <c r="R31" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="B32" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>194</v>
       </c>
       <c r="D32" s="12"/>
@@ -2272,22 +2275,22 @@
         <v>195</v>
       </c>
       <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
       <c r="R32" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>197</v>
       </c>
       <c r="D33" s="12"/>
@@ -2300,22 +2303,22 @@
         <v>198</v>
       </c>
       <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
       <c r="R33" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>200</v>
       </c>
       <c r="D34" s="12"/>
@@ -2328,22 +2331,22 @@
         <v>201</v>
       </c>
       <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="16"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>203</v>
       </c>
       <c r="D35" s="12"/>
@@ -2356,22 +2359,22 @@
         <v>204</v>
       </c>
       <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
       <c r="R35" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>206</v>
       </c>
       <c r="D36" s="12"/>
@@ -2384,22 +2387,22 @@
         <v>207</v>
       </c>
       <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
       <c r="R36" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="7" t="s">
         <v>210</v>
       </c>
       <c r="D37" s="12"/>
@@ -2412,22 +2415,22 @@
         <v>211</v>
       </c>
       <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
       <c r="R37" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="7" t="s">
         <v>213</v>
       </c>
       <c r="D38" s="12"/>
@@ -2440,22 +2443,22 @@
         <v>214</v>
       </c>
       <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
       <c r="R38" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D39" s="12"/>
@@ -2468,12 +2471,12 @@
         <v>217</v>
       </c>
       <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
       <c r="R39" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added e_cell , addmission team
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/005.xlsx
+++ b/docs/STAFF-DATA/005.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="221">
   <si>
     <t>Name</t>
   </si>
@@ -277,6 +277,24 @@
     <t>VEC-005-04-100</t>
   </si>
   <si>
+    <t>Dr. KAVITHA M</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/005/VEC-005-04-611.webp</t>
+  </si>
+  <si>
+    <t>VEC-005-04-611</t>
+  </si>
+  <si>
+    <t>Dr. ALMELU S</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/005/VEC-005-04-720.webp</t>
+  </si>
+  <si>
+    <t>VEC-005-004-720</t>
+  </si>
+  <si>
     <t>Mrs. BHARATHI SHRI C</t>
   </si>
   <si>
@@ -581,15 +599,6 @@
   </si>
   <si>
     <t>VEC-005-04-134</t>
-  </si>
-  <si>
-    <t>Dr. KAVITHA M</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/005/VEC-005-04-611.webp</t>
-  </si>
-  <si>
-    <t>VEC-005-04-611</t>
   </si>
   <si>
     <t>Mrs. GEETHA S</t>
@@ -697,6 +706,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -711,12 +726,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFce9178"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -797,13 +806,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -812,25 +821,25 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -840,10 +849,10 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,7 +1156,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1156,21 +1165,21 @@
     <col min="1" max="1" style="17" width="29.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="18" width="19.14785714285714" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="18" width="53.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="19" width="36.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="20" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="36.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="19" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="48">
@@ -1272,17 +1281,17 @@
       <c r="J3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="88.5">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1339,7 +1348,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="12"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="4" t="s">
         <v>39</v>
       </c>
@@ -1373,7 +1382,7 @@
         <v>44</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="4" t="s">
         <v>45</v>
       </c>
@@ -1405,7 +1414,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="4" t="s">
         <v>50</v>
       </c>
@@ -1477,7 +1486,7 @@
         <v>64</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="4" t="s">
         <v>65</v>
       </c>
@@ -1511,7 +1520,7 @@
         <v>70</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="12"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="4" t="s">
         <v>71</v>
       </c>
@@ -1543,7 +1552,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="4" t="s">
         <v>76</v>
       </c>
@@ -1560,7 +1569,7 @@
       <c r="R11" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33.75">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1581,7 +1590,7 @@
       <c r="G12" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="4" t="s">
         <v>84</v>
       </c>
@@ -1597,8 +1606,8 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33.75">
-      <c r="A13" s="6" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1607,26 +1616,14 @@
       <c r="C13" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="5"/>
@@ -1637,66 +1634,64 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="116.25">
-      <c r="A14" s="13" t="s">
-        <v>92</v>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>94</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D14" s="7"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="4" t="s">
+      <c r="H14" s="7"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="33.75">
+      <c r="A15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="G15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="88.5">
-      <c r="A15" s="6" t="s">
+      <c r="J15" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="5"/>
@@ -1707,36 +1702,28 @@
       <c r="Q15" s="5"/>
       <c r="R15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="13" t="s">
-        <v>105</v>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="116.25">
+      <c r="A16" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>107</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="5"/>
@@ -1747,34 +1734,34 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="88.5">
       <c r="A17" s="6" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="5"/>
@@ -1785,32 +1772,36 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="6" t="s">
-        <v>118</v>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14" t="s">
-        <v>123</v>
+        <v>114</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="5"/>
@@ -1823,26 +1814,32 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="12"/>
+      <c r="F19" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="I19" s="4" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="5"/>
@@ -1855,30 +1852,30 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="5"/>
@@ -1891,26 +1888,26 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="12"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="5"/>
@@ -1923,30 +1920,30 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="5"/>
@@ -1959,32 +1956,26 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>153</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="H23" s="7"/>
       <c r="I23" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="5"/>
@@ -1997,26 +1988,30 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+        <v>150</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>152</v>
+      </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="5"/>
@@ -2029,30 +2024,32 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="5"/>
@@ -2064,27 +2061,27 @@
       <c r="R25" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="13" t="s">
-        <v>169</v>
+      <c r="A26" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="12"/>
+      <c r="H26" s="7"/>
       <c r="I26" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="5"/>
@@ -2096,27 +2093,31 @@
       <c r="R26" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="J27" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>176</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="5"/>
@@ -2128,37 +2129,29 @@
       <c r="R27" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="J28" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="K28" s="10"/>
+      <c r="K28" s="4"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
@@ -2168,27 +2161,27 @@
       <c r="R28" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="6" t="s">
-        <v>182</v>
+      <c r="A29" s="12" t="s">
+        <v>179</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>184</v>
+        <v>84</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="12"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="5"/>
@@ -2200,25 +2193,37 @@
       <c r="R29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K30" s="4"/>
+      <c r="K30" s="10"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
@@ -2228,21 +2233,25 @@
       <c r="R30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D31" s="12"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="4"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="J31" s="4" t="s">
         <v>192</v>
       </c>
@@ -2256,7 +2265,7 @@
       <c r="R31" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>193</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -2265,11 +2274,11 @@
       <c r="C32" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="7"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="12"/>
+      <c r="H32" s="7"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
         <v>195</v>
@@ -2284,7 +2293,7 @@
       <c r="R32" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>196</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -2293,11 +2302,11 @@
       <c r="C33" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="7"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="12"/>
+      <c r="H33" s="7"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
         <v>198</v>
@@ -2311,8 +2320,8 @@
       <c r="Q33" s="5"/>
       <c r="R33" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="13" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="A34" s="12" t="s">
         <v>199</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -2321,11 +2330,11 @@
       <c r="C34" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="D34" s="12"/>
+      <c r="D34" s="7"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="12"/>
+      <c r="H34" s="7"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
         <v>201</v>
@@ -2337,10 +2346,10 @@
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
-      <c r="R34" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="13" t="s">
+      <c r="R34" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+      <c r="A35" s="12" t="s">
         <v>202</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -2349,11 +2358,11 @@
       <c r="C35" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="D35" s="12"/>
+      <c r="D35" s="7"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="12"/>
+      <c r="H35" s="7"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
         <v>204</v>
@@ -2365,10 +2374,10 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
-      <c r="R35" s="4"/>
+      <c r="R35" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>205</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -2377,11 +2386,11 @@
       <c r="C36" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="7"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="12"/>
+      <c r="H36" s="7"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
         <v>207</v>
@@ -2396,23 +2405,23 @@
       <c r="R36" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="12" t="s">
         <v>208</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="7"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="12"/>
+      <c r="H37" s="7"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="5"/>
@@ -2425,19 +2434,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D38" s="12"/>
+      <c r="D38" s="7"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="12"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4" t="s">
         <v>214</v>
@@ -2456,16 +2465,16 @@
         <v>215</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="D39" s="12"/>
+      <c r="D39" s="7"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="12"/>
+      <c r="H39" s="7"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
         <v>217</v>
@@ -2479,6 +2488,34 @@
       <c r="Q39" s="5"/>
       <c r="R39" s="4"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+      <c r="A40" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="K40" s="4"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>